<commit_message>
uploader with image path
</commit_message>
<xml_diff>
--- a/var/import/1.xlsx
+++ b/var/import/1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>category_ids</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>/pdc.png</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -128,7 +125,16 @@
     <t>Default</t>
   </si>
   <si>
-    <t>ELEGANCE GOLD LONG LASTING LIP STICK 8 PINK</t>
+    <t>https://www.pdcorders.com/media/import/pdc.png</t>
+  </si>
+  <si>
+    <t>ELEGANCE GOLD LONG LASTING LIP STICK 9 MAROON</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Catalog, Search</t>
   </si>
 </sst>
 </file>
@@ -531,10 +537,10 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>7155</v>
+        <v>4554</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -561,13 +567,13 @@
         <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="N2">
         <v>100000</v>
@@ -582,28 +588,28 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
         <v>29</v>
-      </c>
-      <c r="S2" t="s">
-        <v>30</v>
       </c>
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>4</v>
+      <c r="U2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
       </c>
       <c r="W2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" t="s">
         <v>31</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>32</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with 3 data to test
</commit_message>
<xml_diff>
--- a/var/import/1.xlsx
+++ b/var/import/1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>category_ids</t>
   </si>
@@ -128,23 +128,37 @@
     <t>https://www.pdcorders.com/media/import/pdc.png</t>
   </si>
   <si>
-    <t>ELEGANCE GOLD LONG LASTING LIP STICK 9 MAROON</t>
-  </si>
-  <si>
-    <t>Enabled</t>
-  </si>
-  <si>
-    <t>Catalog, Search</t>
+    <t>ELEGANCE GOLD MATIC EYE CONTOUR BLACK</t>
+  </si>
+  <si>
+    <t>ELEGANCE GOLD MATIC EYE CONTOUR BROWN</t>
+  </si>
+  <si>
+    <t>media/import/pdc.png</t>
+  </si>
+  <si>
+    <t>ELEGANCE GOLD SOFT SHINY EYE LINER BLACK</t>
+  </si>
+  <si>
+    <t>/home/pdcorders.com/media/import/pdc.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,13 +181,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,9 +469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -537,10 +556,10 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>4554</v>
+        <v>6972</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -566,13 +585,13 @@
       <c r="J2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N2">
@@ -596,11 +615,11 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="U2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" t="s">
-        <v>36</v>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>4</v>
       </c>
       <c r="W2" t="s">
         <v>30</v>
@@ -612,7 +631,166 @@
         <v>32</v>
       </c>
     </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>6974</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3">
+        <v>100000</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+      <c r="W3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>7156</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4">
+        <v>100000</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>4</v>
+      </c>
+      <c r="W4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId2"/>
+    <hyperlink ref="M2" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated with test excel
</commit_message>
<xml_diff>
--- a/var/import/1.xlsx
+++ b/var/import/1.xlsx
@@ -128,13 +128,13 @@
     <t>MODERN PHARMACEUTICAL CO.</t>
   </si>
   <si>
-    <t>ELEGANCE LASTING LIP STICK 6</t>
-  </si>
-  <si>
-    <t>ELEGANCE LINE SHADOW POWDER 1</t>
-  </si>
-  <si>
     <t>ELEMENT MIDDLE EAST LLC</t>
+  </si>
+  <si>
+    <t>ELEGANCE LINE SHADOW POWDER 2</t>
+  </si>
+  <si>
+    <t>ELEGANCE LINE SHADOW POWDER 3</t>
   </si>
 </sst>
 </file>
@@ -537,16 +537,16 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>7159</v>
+        <v>2987</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -561,10 +561,10 @@
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K2" t="s">
         <v>32</v>
@@ -617,13 +617,13 @@
         <v>19</v>
       </c>
       <c r="B3">
-        <v>2986</v>
+        <v>2988</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -632,16 +632,16 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
import reverted for check
</commit_message>
<xml_diff>
--- a/var/import/1.xlsx
+++ b/var/import/1.xlsx
@@ -128,10 +128,10 @@
     <t>MODERN PHARMACEUTICAL CO.</t>
   </si>
   <si>
-    <t>ELEGANCE LINE SHADOW POWDER 4</t>
-  </si>
-  <si>
-    <t>ELEGANCE LIP CONTOUR 2035 NUDE BROWN</t>
+    <t>ELEGANCE LIP CONTOUR 2044 ORANGE</t>
+  </si>
+  <si>
+    <t>ELEGANCE LIP CONTOUR BROWN</t>
   </si>
 </sst>
 </file>
@@ -534,10 +534,10 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>2989</v>
+        <v>7161</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -611,10 +611,10 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>7160</v>
+        <v>7162</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>

</xml_diff>